<commit_message>
:sparkles: Mudando TransactionItem para String
</commit_message>
<xml_diff>
--- a/GenerateYearlyReportDispatcher/Data/Config.xlsx
+++ b/GenerateYearlyReportDispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Documents\GitHub\UiPath\GenerateYearlyReportDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A21922-18CC-4C93-B9F9-9F3DCA448ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62681D4-327F-4D7D-A169-D6EB5E65DD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1650" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="1650" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1689,7 +1689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
:sparkles: Quase concluindo o Dispatcher
</commit_message>
<xml_diff>
--- a/GenerateYearlyReportDispatcher/Data/Config.xlsx
+++ b/GenerateYearlyReportDispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Documents\GitHub\UiPath\GenerateYearlyReportDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62681D4-327F-4D7D-A169-D6EB5E65DD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06287E2D-6280-4816-9513-781A52B69010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3630" yWindow="1650" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>